<commit_message>
corrigido metodo get ultima data
</commit_message>
<xml_diff>
--- a/bases/precos_cacau_ilheus.xlsx
+++ b/bases/precos_cacau_ilheus.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="1760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="1869">
   <si>
     <t>vr_real</t>
   </si>
@@ -5294,6 +5294,333 @@
   </si>
   <si>
     <t>2018-04-05</t>
+  </si>
+  <si>
+    <t>2018-04-25</t>
+  </si>
+  <si>
+    <t>2018-04-26</t>
+  </si>
+  <si>
+    <t>2018-04-27</t>
+  </si>
+  <si>
+    <t>2018-05-02</t>
+  </si>
+  <si>
+    <t>2018-05-03</t>
+  </si>
+  <si>
+    <t>2018-05-04</t>
+  </si>
+  <si>
+    <t>2018-05-07</t>
+  </si>
+  <si>
+    <t>2018-05-08</t>
+  </si>
+  <si>
+    <t>2018-05-09</t>
+  </si>
+  <si>
+    <t>2018-05-10</t>
+  </si>
+  <si>
+    <t>2018-05-11</t>
+  </si>
+  <si>
+    <t>2018-05-14</t>
+  </si>
+  <si>
+    <t>2018-05-15</t>
+  </si>
+  <si>
+    <t>2018-05-16</t>
+  </si>
+  <si>
+    <t>2018-05-17</t>
+  </si>
+  <si>
+    <t>2018-05-18</t>
+  </si>
+  <si>
+    <t>2018-05-21</t>
+  </si>
+  <si>
+    <t>2018-05-22</t>
+  </si>
+  <si>
+    <t>2018-05-23</t>
+  </si>
+  <si>
+    <t>2018-05-24</t>
+  </si>
+  <si>
+    <t>2018-05-25</t>
+  </si>
+  <si>
+    <t>2018-05-28</t>
+  </si>
+  <si>
+    <t>2018-05-29</t>
+  </si>
+  <si>
+    <t>2018-05-30</t>
+  </si>
+  <si>
+    <t>2018-06-04</t>
+  </si>
+  <si>
+    <t>2018-06-05</t>
+  </si>
+  <si>
+    <t>2018-06-06</t>
+  </si>
+  <si>
+    <t>2018-06-08</t>
+  </si>
+  <si>
+    <t>2018-06-11</t>
+  </si>
+  <si>
+    <t>2018-06-12</t>
+  </si>
+  <si>
+    <t>2018-06-13</t>
+  </si>
+  <si>
+    <t>2018-06-14</t>
+  </si>
+  <si>
+    <t>2018-06-15</t>
+  </si>
+  <si>
+    <t>2018-06-18</t>
+  </si>
+  <si>
+    <t>2018-06-19</t>
+  </si>
+  <si>
+    <t>2018-06-20</t>
+  </si>
+  <si>
+    <t>2018-06-21</t>
+  </si>
+  <si>
+    <t>2018-06-25</t>
+  </si>
+  <si>
+    <t>2018-06-26</t>
+  </si>
+  <si>
+    <t>2018-06-27</t>
+  </si>
+  <si>
+    <t>2018-06-29</t>
+  </si>
+  <si>
+    <t>2018-07-03</t>
+  </si>
+  <si>
+    <t>2018-07-04</t>
+  </si>
+  <si>
+    <t>2018-07-05</t>
+  </si>
+  <si>
+    <t>2018-07-06</t>
+  </si>
+  <si>
+    <t>2018-07-09</t>
+  </si>
+  <si>
+    <t>2018-07-10</t>
+  </si>
+  <si>
+    <t>2018-07-11</t>
+  </si>
+  <si>
+    <t>2018-07-12</t>
+  </si>
+  <si>
+    <t>2018-07-13</t>
+  </si>
+  <si>
+    <t>2018-07-16</t>
+  </si>
+  <si>
+    <t>2018-07-17</t>
+  </si>
+  <si>
+    <t>2018-07-18</t>
+  </si>
+  <si>
+    <t>2018-07-19</t>
+  </si>
+  <si>
+    <t>2018-07-20</t>
+  </si>
+  <si>
+    <t>2018-07-23</t>
+  </si>
+  <si>
+    <t>2018-07-24</t>
+  </si>
+  <si>
+    <t>2018-07-25</t>
+  </si>
+  <si>
+    <t>2018-07-26</t>
+  </si>
+  <si>
+    <t>2018-07-27</t>
+  </si>
+  <si>
+    <t>2018-07-30</t>
+  </si>
+  <si>
+    <t>2018-07-31</t>
+  </si>
+  <si>
+    <t>2018-08-01</t>
+  </si>
+  <si>
+    <t>2018-08-02</t>
+  </si>
+  <si>
+    <t>2018-08-03</t>
+  </si>
+  <si>
+    <t>2018-08-06</t>
+  </si>
+  <si>
+    <t>2018-08-07</t>
+  </si>
+  <si>
+    <t>2018-08-08</t>
+  </si>
+  <si>
+    <t>2018-08-09</t>
+  </si>
+  <si>
+    <t>2018-08-10</t>
+  </si>
+  <si>
+    <t>2018-08-13</t>
+  </si>
+  <si>
+    <t>2018-08-14</t>
+  </si>
+  <si>
+    <t>2018-08-15</t>
+  </si>
+  <si>
+    <t>2018-08-16</t>
+  </si>
+  <si>
+    <t>2018-08-17</t>
+  </si>
+  <si>
+    <t>2018-08-20</t>
+  </si>
+  <si>
+    <t>2018-08-21</t>
+  </si>
+  <si>
+    <t>2018-08-22</t>
+  </si>
+  <si>
+    <t>2018-08-23</t>
+  </si>
+  <si>
+    <t>2018-08-24</t>
+  </si>
+  <si>
+    <t>2018-08-27</t>
+  </si>
+  <si>
+    <t>2018-08-28</t>
+  </si>
+  <si>
+    <t>2018-08-29</t>
+  </si>
+  <si>
+    <t>2018-08-30</t>
+  </si>
+  <si>
+    <t>2018-08-31</t>
+  </si>
+  <si>
+    <t>2018-09-03</t>
+  </si>
+  <si>
+    <t>2018-09-04</t>
+  </si>
+  <si>
+    <t>2018-09-05</t>
+  </si>
+  <si>
+    <t>2018-09-06</t>
+  </si>
+  <si>
+    <t>2018-09-10</t>
+  </si>
+  <si>
+    <t>2018-09-11</t>
+  </si>
+  <si>
+    <t>2018-09-12</t>
+  </si>
+  <si>
+    <t>2018-09-13</t>
+  </si>
+  <si>
+    <t>2018-09-14</t>
+  </si>
+  <si>
+    <t>2018-09-17</t>
+  </si>
+  <si>
+    <t>2018-09-18</t>
+  </si>
+  <si>
+    <t>2018-09-19</t>
+  </si>
+  <si>
+    <t>2018-09-20</t>
+  </si>
+  <si>
+    <t>2018-09-21</t>
+  </si>
+  <si>
+    <t>2018-09-24</t>
+  </si>
+  <si>
+    <t>2018-09-25</t>
+  </si>
+  <si>
+    <t>2018-09-26</t>
+  </si>
+  <si>
+    <t>2018-09-27</t>
+  </si>
+  <si>
+    <t>2018-09-28</t>
+  </si>
+  <si>
+    <t>2018-10-01</t>
+  </si>
+  <si>
+    <t>2018-10-02</t>
+  </si>
+  <si>
+    <t>2018-10-03</t>
+  </si>
+  <si>
+    <t>2018-10-04</t>
+  </si>
+  <si>
+    <t>2018-10-05</t>
   </si>
 </sst>
 </file>
@@ -5651,7 +5978,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1765"/>
+  <dimension ref="A1:G1874"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -45810,6 +46137,2513 @@
       <c r="E1765">
         <v>118.25</v>
       </c>
+      <c r="F1765">
+        <v>-2.54</v>
+      </c>
+      <c r="G1765">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:7">
+      <c r="A1766" s="1" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B1766">
+        <v>175</v>
+      </c>
+      <c r="C1766">
+        <v>131.33</v>
+      </c>
+      <c r="D1766">
+        <v>126.43</v>
+      </c>
+      <c r="E1766">
+        <v>119.37</v>
+      </c>
+      <c r="F1766">
+        <v>-2.65</v>
+      </c>
+      <c r="G1766">
+        <v>-1.57</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:7">
+      <c r="A1767" s="1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B1767">
+        <v>178.5</v>
+      </c>
+      <c r="C1767">
+        <v>134.9</v>
+      </c>
+      <c r="D1767">
+        <v>128.45</v>
+      </c>
+      <c r="E1767">
+        <v>120.54</v>
+      </c>
+      <c r="F1767">
+        <v>-2.23</v>
+      </c>
+      <c r="G1767">
+        <v>-1.33</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:7">
+      <c r="A1768" s="1" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B1768">
+        <v>171</v>
+      </c>
+      <c r="C1768">
+        <v>137.97</v>
+      </c>
+      <c r="D1768">
+        <v>130.18</v>
+      </c>
+      <c r="E1768">
+        <v>121.58</v>
+      </c>
+      <c r="F1768">
+        <v>-2.52</v>
+      </c>
+      <c r="G1768">
+        <v>-1.51</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:7">
+      <c r="A1769" s="1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B1769">
+        <v>178.65</v>
+      </c>
+      <c r="C1769">
+        <v>141.54</v>
+      </c>
+      <c r="D1769">
+        <v>132.17</v>
+      </c>
+      <c r="E1769">
+        <v>122.72</v>
+      </c>
+      <c r="F1769">
+        <v>-2.44</v>
+      </c>
+      <c r="G1769">
+        <v>-1.47</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:7">
+      <c r="A1770" s="1" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B1770">
+        <v>178</v>
+      </c>
+      <c r="C1770">
+        <v>145.08</v>
+      </c>
+      <c r="D1770">
+        <v>134.14</v>
+      </c>
+      <c r="E1770">
+        <v>123.85</v>
+      </c>
+      <c r="F1770">
+        <v>-2.4</v>
+      </c>
+      <c r="G1770">
+        <v>-1.45</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:7">
+      <c r="A1771" s="1" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B1771">
+        <v>178.5</v>
+      </c>
+      <c r="C1771">
+        <v>148.64</v>
+      </c>
+      <c r="D1771">
+        <v>136.12</v>
+      </c>
+      <c r="E1771">
+        <v>124.99</v>
+      </c>
+      <c r="F1771">
+        <v>-2.33</v>
+      </c>
+      <c r="G1771">
+        <v>-1.4</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:7">
+      <c r="A1772" s="1" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B1772">
+        <v>178</v>
+      </c>
+      <c r="C1772">
+        <v>152.18</v>
+      </c>
+      <c r="D1772">
+        <v>138.05</v>
+      </c>
+      <c r="E1772">
+        <v>126.13</v>
+      </c>
+      <c r="F1772">
+        <v>-2.19</v>
+      </c>
+      <c r="G1772">
+        <v>-1.39</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:7">
+      <c r="A1773" s="1" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B1773">
+        <v>179</v>
+      </c>
+      <c r="C1773">
+        <v>155.58</v>
+      </c>
+      <c r="D1773">
+        <v>139.99</v>
+      </c>
+      <c r="E1773">
+        <v>127.26</v>
+      </c>
+      <c r="F1773">
+        <v>-1.89</v>
+      </c>
+      <c r="G1773">
+        <v>-1.27</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:7">
+      <c r="A1774" s="1" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B1774">
+        <v>175</v>
+      </c>
+      <c r="C1774">
+        <v>158.58</v>
+      </c>
+      <c r="D1774">
+        <v>141.79</v>
+      </c>
+      <c r="E1774">
+        <v>128.33</v>
+      </c>
+      <c r="F1774">
+        <v>-1.98</v>
+      </c>
+      <c r="G1774">
+        <v>-1.23</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:7">
+      <c r="A1775" s="1" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B1775">
+        <v>175</v>
+      </c>
+      <c r="C1775">
+        <v>161.78</v>
+      </c>
+      <c r="D1775">
+        <v>143.55</v>
+      </c>
+      <c r="E1775">
+        <v>129.38</v>
+      </c>
+      <c r="F1775">
+        <v>-1.82</v>
+      </c>
+      <c r="G1775">
+        <v>-1.22</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:7">
+      <c r="A1776" s="1" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B1776">
+        <v>175</v>
+      </c>
+      <c r="C1776">
+        <v>164.78</v>
+      </c>
+      <c r="D1776">
+        <v>145.32</v>
+      </c>
+      <c r="E1776">
+        <v>130.44</v>
+      </c>
+      <c r="F1776">
+        <v>-1.98</v>
+      </c>
+      <c r="G1776">
+        <v>-1.27</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:7">
+      <c r="A1777" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B1777">
+        <v>180</v>
+      </c>
+      <c r="C1777">
+        <v>168.11</v>
+      </c>
+      <c r="D1777">
+        <v>147.19</v>
+      </c>
+      <c r="E1777">
+        <v>131.63</v>
+      </c>
+      <c r="F1777">
+        <v>-1.98</v>
+      </c>
+      <c r="G1777">
+        <v>-1.27</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:7">
+      <c r="A1778" s="1" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B1778">
+        <v>181</v>
+      </c>
+      <c r="C1778">
+        <v>171.51</v>
+      </c>
+      <c r="D1778">
+        <v>149.09</v>
+      </c>
+      <c r="E1778">
+        <v>132.81</v>
+      </c>
+      <c r="F1778">
+        <v>-1.53</v>
+      </c>
+      <c r="G1778">
+        <v>-1.11</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:7">
+      <c r="A1779" s="1" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B1779">
+        <v>175</v>
+      </c>
+      <c r="C1779">
+        <v>174.18</v>
+      </c>
+      <c r="D1779">
+        <v>150.76</v>
+      </c>
+      <c r="E1779">
+        <v>133.89</v>
+      </c>
+      <c r="F1779">
+        <v>-1.65</v>
+      </c>
+      <c r="G1779">
+        <v>-1.17</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:7">
+      <c r="A1780" s="1" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B1780">
+        <v>179</v>
+      </c>
+      <c r="C1780">
+        <v>177.11</v>
+      </c>
+      <c r="D1780">
+        <v>152.55</v>
+      </c>
+      <c r="E1780">
+        <v>135.04</v>
+      </c>
+      <c r="F1780">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="G1780">
+        <v>-1.13</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:7">
+      <c r="A1781" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B1781">
+        <v>177</v>
+      </c>
+      <c r="C1781">
+        <v>177.24</v>
+      </c>
+      <c r="D1781">
+        <v>154.29</v>
+      </c>
+      <c r="E1781">
+        <v>136.16</v>
+      </c>
+      <c r="F1781">
+        <v>-0.02</v>
+      </c>
+      <c r="G1781">
+        <v>-1.15</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:7">
+      <c r="A1782" s="1" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B1782">
+        <v>179</v>
+      </c>
+      <c r="C1782">
+        <v>177.28</v>
+      </c>
+      <c r="D1782">
+        <v>156.09</v>
+      </c>
+      <c r="E1782">
+        <v>137.29</v>
+      </c>
+      <c r="F1782">
+        <v>-0.15</v>
+      </c>
+      <c r="G1782">
+        <v>-1.06</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:7">
+      <c r="A1783" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B1783">
+        <v>175</v>
+      </c>
+      <c r="C1783">
+        <v>177.54</v>
+      </c>
+      <c r="D1783">
+        <v>157.76</v>
+      </c>
+      <c r="E1783">
+        <v>138.38</v>
+      </c>
+      <c r="F1783">
+        <v>0.14</v>
+      </c>
+      <c r="G1783">
+        <v>-1.04</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:7">
+      <c r="A1784" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B1784">
+        <v>175</v>
+      </c>
+      <c r="C1784">
+        <v>177.3</v>
+      </c>
+      <c r="D1784">
+        <v>159.42</v>
+      </c>
+      <c r="E1784">
+        <v>139.44</v>
+      </c>
+      <c r="F1784">
+        <v>0.11</v>
+      </c>
+      <c r="G1784">
+        <v>-1.04</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:7">
+      <c r="A1785" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B1785">
+        <v>175</v>
+      </c>
+      <c r="C1785">
+        <v>177.1</v>
+      </c>
+      <c r="D1785">
+        <v>161.09</v>
+      </c>
+      <c r="E1785">
+        <v>140.49</v>
+      </c>
+      <c r="F1785">
+        <v>0.15</v>
+      </c>
+      <c r="G1785">
+        <v>-1.01</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:7">
+      <c r="A1786" s="1" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B1786">
+        <v>174.5</v>
+      </c>
+      <c r="C1786">
+        <v>176.83</v>
+      </c>
+      <c r="D1786">
+        <v>162.74</v>
+      </c>
+      <c r="E1786">
+        <v>141.52</v>
+      </c>
+      <c r="F1786">
+        <v>0.19</v>
+      </c>
+      <c r="G1786">
+        <v>-0.97</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:7">
+      <c r="A1787" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B1787">
+        <v>173</v>
+      </c>
+      <c r="C1787">
+        <v>176.5</v>
+      </c>
+      <c r="D1787">
+        <v>164.34</v>
+      </c>
+      <c r="E1787">
+        <v>142.49</v>
+      </c>
+      <c r="F1787">
+        <v>0.1</v>
+      </c>
+      <c r="G1787">
+        <v>-0.98</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:7">
+      <c r="A1788" s="1" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B1788">
+        <v>176.5</v>
+      </c>
+      <c r="C1788">
+        <v>176.33</v>
+      </c>
+      <c r="D1788">
+        <v>165.96</v>
+      </c>
+      <c r="E1788">
+        <v>143.51</v>
+      </c>
+      <c r="F1788">
+        <v>0.15</v>
+      </c>
+      <c r="G1788">
+        <v>-0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:7">
+      <c r="A1789" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B1789">
+        <v>171</v>
+      </c>
+      <c r="C1789">
+        <v>176.07</v>
+      </c>
+      <c r="D1789">
+        <v>167.32</v>
+      </c>
+      <c r="E1789">
+        <v>144.44</v>
+      </c>
+      <c r="F1789">
+        <v>0.27</v>
+      </c>
+      <c r="G1789">
+        <v>-0.8100000000000001</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:7">
+      <c r="A1790" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B1790">
+        <v>168</v>
+      </c>
+      <c r="C1790">
+        <v>175.6</v>
+      </c>
+      <c r="D1790">
+        <v>168.69</v>
+      </c>
+      <c r="E1790">
+        <v>145.33</v>
+      </c>
+      <c r="F1790">
+        <v>0.42</v>
+      </c>
+      <c r="G1790">
+        <v>-0.67</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:7">
+      <c r="A1791" s="1" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B1791">
+        <v>164</v>
+      </c>
+      <c r="C1791">
+        <v>174.87</v>
+      </c>
+      <c r="D1791">
+        <v>169.82</v>
+      </c>
+      <c r="E1791">
+        <v>146.14</v>
+      </c>
+      <c r="F1791">
+        <v>0.58</v>
+      </c>
+      <c r="G1791">
+        <v>-0.68</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:7">
+      <c r="A1792" s="1" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B1792">
+        <v>165</v>
+      </c>
+      <c r="C1792">
+        <v>173.87</v>
+      </c>
+      <c r="D1792">
+        <v>170.99</v>
+      </c>
+      <c r="E1792">
+        <v>146.94</v>
+      </c>
+      <c r="F1792">
+        <v>0.74</v>
+      </c>
+      <c r="G1792">
+        <v>-0.62</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:7">
+      <c r="A1793" s="1" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B1793">
+        <v>162</v>
+      </c>
+      <c r="C1793">
+        <v>172.6</v>
+      </c>
+      <c r="D1793">
+        <v>172.05</v>
+      </c>
+      <c r="E1793">
+        <v>147.69</v>
+      </c>
+      <c r="F1793">
+        <v>0.54</v>
+      </c>
+      <c r="G1793">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:7">
+      <c r="A1794" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B1794">
+        <v>161</v>
+      </c>
+      <c r="C1794">
+        <v>171.67</v>
+      </c>
+      <c r="D1794">
+        <v>172.92</v>
+      </c>
+      <c r="E1794">
+        <v>148.43</v>
+      </c>
+      <c r="F1794">
+        <v>0.67</v>
+      </c>
+      <c r="G1794">
+        <v>-0.52</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:7">
+      <c r="A1795" s="1" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B1795">
+        <v>162</v>
+      </c>
+      <c r="C1795">
+        <v>170.53</v>
+      </c>
+      <c r="D1795">
+        <v>173.82</v>
+      </c>
+      <c r="E1795">
+        <v>149.18</v>
+      </c>
+      <c r="F1795">
+        <v>0.63</v>
+      </c>
+      <c r="G1795">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:7">
+      <c r="A1796" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B1796">
+        <v>161</v>
+      </c>
+      <c r="C1796">
+        <v>169.47</v>
+      </c>
+      <c r="D1796">
+        <v>173.36</v>
+      </c>
+      <c r="E1796">
+        <v>149.89</v>
+      </c>
+      <c r="F1796">
+        <v>0.7</v>
+      </c>
+      <c r="G1796">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:7">
+      <c r="A1797" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1797">
+        <v>161.5</v>
+      </c>
+      <c r="C1797">
+        <v>168.3</v>
+      </c>
+      <c r="D1797">
+        <v>172.79</v>
+      </c>
+      <c r="E1797">
+        <v>150.62</v>
+      </c>
+      <c r="F1797">
+        <v>0.48</v>
+      </c>
+      <c r="G1797">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:7">
+      <c r="A1798" s="1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B1798">
+        <v>163</v>
+      </c>
+      <c r="C1798">
+        <v>167.5</v>
+      </c>
+      <c r="D1798">
+        <v>172.52</v>
+      </c>
+      <c r="E1798">
+        <v>151.35</v>
+      </c>
+      <c r="F1798">
+        <v>0.36</v>
+      </c>
+      <c r="G1798">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:7">
+      <c r="A1799" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B1799">
+        <v>166</v>
+      </c>
+      <c r="C1799">
+        <v>166.9</v>
+      </c>
+      <c r="D1799">
+        <v>172.1</v>
+      </c>
+      <c r="E1799">
+        <v>152.14</v>
+      </c>
+      <c r="F1799">
+        <v>0.34</v>
+      </c>
+      <c r="G1799">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:7">
+      <c r="A1800" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B1800">
+        <v>166.5</v>
+      </c>
+      <c r="C1800">
+        <v>166.33</v>
+      </c>
+      <c r="D1800">
+        <v>171.72</v>
+      </c>
+      <c r="E1800">
+        <v>152.93</v>
+      </c>
+      <c r="F1800">
+        <v>0.34</v>
+      </c>
+      <c r="G1800">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:7">
+      <c r="A1801" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B1801">
+        <v>166</v>
+      </c>
+      <c r="C1801">
+        <v>165.77</v>
+      </c>
+      <c r="D1801">
+        <v>171.3</v>
+      </c>
+      <c r="E1801">
+        <v>153.71</v>
+      </c>
+      <c r="F1801">
+        <v>0.28</v>
+      </c>
+      <c r="G1801">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:7">
+      <c r="A1802" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B1802">
+        <v>166</v>
+      </c>
+      <c r="C1802">
+        <v>165.3</v>
+      </c>
+      <c r="D1802">
+        <v>170.9</v>
+      </c>
+      <c r="E1802">
+        <v>154.48</v>
+      </c>
+      <c r="F1802">
+        <v>0.47</v>
+      </c>
+      <c r="G1802">
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:7">
+      <c r="A1803" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B1803">
+        <v>165</v>
+      </c>
+      <c r="C1803">
+        <v>164.53</v>
+      </c>
+      <c r="D1803">
+        <v>170.43</v>
+      </c>
+      <c r="E1803">
+        <v>155.21</v>
+      </c>
+      <c r="F1803">
+        <v>0.32</v>
+      </c>
+      <c r="G1803">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:7">
+      <c r="A1804" s="1" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B1804">
+        <v>163</v>
+      </c>
+      <c r="C1804">
+        <v>164</v>
+      </c>
+      <c r="D1804">
+        <v>170.03</v>
+      </c>
+      <c r="E1804">
+        <v>155.91</v>
+      </c>
+      <c r="F1804">
+        <v>0.32</v>
+      </c>
+      <c r="G1804">
+        <v>0.29</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:7">
+      <c r="A1805" s="1" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B1805">
+        <v>160</v>
+      </c>
+      <c r="C1805">
+        <v>163.47</v>
+      </c>
+      <c r="D1805">
+        <v>169.53</v>
+      </c>
+      <c r="E1805">
+        <v>156.54</v>
+      </c>
+      <c r="F1805">
+        <v>0.09</v>
+      </c>
+      <c r="G1805">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:7">
+      <c r="A1806" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B1806">
+        <v>162</v>
+      </c>
+      <c r="C1806">
+        <v>163.33</v>
+      </c>
+      <c r="D1806">
+        <v>169.1</v>
+      </c>
+      <c r="E1806">
+        <v>157.21</v>
+      </c>
+      <c r="F1806">
+        <v>0.06</v>
+      </c>
+      <c r="G1806">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:7">
+      <c r="A1807" s="1" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B1807">
+        <v>163.5</v>
+      </c>
+      <c r="C1807">
+        <v>163.23</v>
+      </c>
+      <c r="D1807">
+        <v>168.55</v>
+      </c>
+      <c r="E1807">
+        <v>157.87</v>
+      </c>
+      <c r="F1807">
+        <v>0.06</v>
+      </c>
+      <c r="G1807">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:7">
+      <c r="A1808" s="1" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B1808">
+        <v>160.5</v>
+      </c>
+      <c r="C1808">
+        <v>163.13</v>
+      </c>
+      <c r="D1808">
+        <v>167.87</v>
+      </c>
+      <c r="E1808">
+        <v>158.48</v>
+      </c>
+      <c r="F1808">
+        <v>0.08</v>
+      </c>
+      <c r="G1808">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:7">
+      <c r="A1809" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B1809">
+        <v>159</v>
+      </c>
+      <c r="C1809">
+        <v>163</v>
+      </c>
+      <c r="D1809">
+        <v>167.33</v>
+      </c>
+      <c r="E1809">
+        <v>159.04</v>
+      </c>
+      <c r="F1809">
+        <v>0.08</v>
+      </c>
+      <c r="G1809">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:7">
+      <c r="A1810" s="1" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B1810">
+        <v>160</v>
+      </c>
+      <c r="C1810">
+        <v>162.87</v>
+      </c>
+      <c r="D1810">
+        <v>166.7</v>
+      </c>
+      <c r="E1810">
+        <v>159.63</v>
+      </c>
+      <c r="F1810">
+        <v>0.09</v>
+      </c>
+      <c r="G1810">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:7">
+      <c r="A1811" s="1" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B1811">
+        <v>159</v>
+      </c>
+      <c r="C1811">
+        <v>162.73</v>
+      </c>
+      <c r="D1811">
+        <v>166.1</v>
+      </c>
+      <c r="E1811">
+        <v>160.19</v>
+      </c>
+      <c r="F1811">
+        <v>0.11</v>
+      </c>
+      <c r="G1811">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:7">
+      <c r="A1812" s="1" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B1812">
+        <v>158.7</v>
+      </c>
+      <c r="C1812">
+        <v>162.55</v>
+      </c>
+      <c r="D1812">
+        <v>165.42</v>
+      </c>
+      <c r="E1812">
+        <v>160.76</v>
+      </c>
+      <c r="F1812">
+        <v>0.34</v>
+      </c>
+      <c r="G1812">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:7">
+      <c r="A1813" s="1" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B1813">
+        <v>154.8</v>
+      </c>
+      <c r="C1813">
+        <v>162</v>
+      </c>
+      <c r="D1813">
+        <v>164.75</v>
+      </c>
+      <c r="E1813">
+        <v>161.25</v>
+      </c>
+      <c r="F1813">
+        <v>0.47</v>
+      </c>
+      <c r="G1813">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:7">
+      <c r="A1814" s="1" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B1814">
+        <v>154.8</v>
+      </c>
+      <c r="C1814">
+        <v>161.25</v>
+      </c>
+      <c r="D1814">
+        <v>164.08</v>
+      </c>
+      <c r="E1814">
+        <v>161.75</v>
+      </c>
+      <c r="F1814">
+        <v>0.42</v>
+      </c>
+      <c r="G1814">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:7">
+      <c r="A1815" s="1" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B1815">
+        <v>156.4</v>
+      </c>
+      <c r="C1815">
+        <v>160.58</v>
+      </c>
+      <c r="D1815">
+        <v>163.46</v>
+      </c>
+      <c r="E1815">
+        <v>162.27</v>
+      </c>
+      <c r="F1815">
+        <v>0.36</v>
+      </c>
+      <c r="G1815">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:7">
+      <c r="A1816" s="1" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B1816">
+        <v>157.5</v>
+      </c>
+      <c r="C1816">
+        <v>160.01</v>
+      </c>
+      <c r="D1816">
+        <v>162.89</v>
+      </c>
+      <c r="E1816">
+        <v>162.81</v>
+      </c>
+      <c r="F1816">
+        <v>0.77</v>
+      </c>
+      <c r="G1816">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:7">
+      <c r="A1817" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B1817">
+        <v>147.5</v>
+      </c>
+      <c r="C1817">
+        <v>158.78</v>
+      </c>
+      <c r="D1817">
+        <v>162.04</v>
+      </c>
+      <c r="E1817">
+        <v>163.19</v>
+      </c>
+      <c r="F1817">
+        <v>0.75</v>
+      </c>
+      <c r="G1817">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:7">
+      <c r="A1818" s="1" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B1818">
+        <v>147.3</v>
+      </c>
+      <c r="C1818">
+        <v>157.6</v>
+      </c>
+      <c r="D1818">
+        <v>161.07</v>
+      </c>
+      <c r="E1818">
+        <v>163.51</v>
+      </c>
+      <c r="F1818">
+        <v>0.77</v>
+      </c>
+      <c r="G1818">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:7">
+      <c r="A1819" s="1" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B1819">
+        <v>145</v>
+      </c>
+      <c r="C1819">
+        <v>156.4</v>
+      </c>
+      <c r="D1819">
+        <v>160.2</v>
+      </c>
+      <c r="E1819">
+        <v>163.76</v>
+      </c>
+      <c r="F1819">
+        <v>0.84</v>
+      </c>
+      <c r="G1819">
+        <v>0.58</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:7">
+      <c r="A1820" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B1820">
+        <v>140.5</v>
+      </c>
+      <c r="C1820">
+        <v>155.1</v>
+      </c>
+      <c r="D1820">
+        <v>159.28</v>
+      </c>
+      <c r="E1820">
+        <v>163.99</v>
+      </c>
+      <c r="F1820">
+        <v>1</v>
+      </c>
+      <c r="G1820">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:7">
+      <c r="A1821" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B1821">
+        <v>139</v>
+      </c>
+      <c r="C1821">
+        <v>153.57</v>
+      </c>
+      <c r="D1821">
+        <v>158.45</v>
+      </c>
+      <c r="E1821">
+        <v>164.14</v>
+      </c>
+      <c r="F1821">
+        <v>1.32</v>
+      </c>
+      <c r="G1821">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:7">
+      <c r="A1822" s="1" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B1822">
+        <v>133.5</v>
+      </c>
+      <c r="C1822">
+        <v>151.57</v>
+      </c>
+      <c r="D1822">
+        <v>157.4</v>
+      </c>
+      <c r="E1822">
+        <v>164.19</v>
+      </c>
+      <c r="F1822">
+        <v>1.34</v>
+      </c>
+      <c r="G1822">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="1823" spans="1:7">
+      <c r="A1823" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1823">
+        <v>130.5</v>
+      </c>
+      <c r="C1823">
+        <v>149.57</v>
+      </c>
+      <c r="D1823">
+        <v>156.35</v>
+      </c>
+      <c r="E1823">
+        <v>164.2</v>
+      </c>
+      <c r="F1823">
+        <v>1.33</v>
+      </c>
+      <c r="G1823">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="1824" spans="1:7">
+      <c r="A1824" s="1" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B1824">
+        <v>129.5</v>
+      </c>
+      <c r="C1824">
+        <v>147.6</v>
+      </c>
+      <c r="D1824">
+        <v>155.3</v>
+      </c>
+      <c r="E1824">
+        <v>164.11</v>
+      </c>
+      <c r="F1824">
+        <v>1.35</v>
+      </c>
+      <c r="G1824">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:7">
+      <c r="A1825" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B1825">
+        <v>130.5</v>
+      </c>
+      <c r="C1825">
+        <v>145.63</v>
+      </c>
+      <c r="D1825">
+        <v>154.25</v>
+      </c>
+      <c r="E1825">
+        <v>164.04</v>
+      </c>
+      <c r="F1825">
+        <v>1.36</v>
+      </c>
+      <c r="G1825">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:7">
+      <c r="A1826" s="1" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B1826">
+        <v>129.5</v>
+      </c>
+      <c r="C1826">
+        <v>143.67</v>
+      </c>
+      <c r="D1826">
+        <v>153.2</v>
+      </c>
+      <c r="E1826">
+        <v>163.28</v>
+      </c>
+      <c r="F1826">
+        <v>1.43</v>
+      </c>
+      <c r="G1826">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="1827" spans="1:7">
+      <c r="A1827" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B1827">
+        <v>128.5</v>
+      </c>
+      <c r="C1827">
+        <v>141.65</v>
+      </c>
+      <c r="D1827">
+        <v>152.1</v>
+      </c>
+      <c r="E1827">
+        <v>162.44</v>
+      </c>
+      <c r="F1827">
+        <v>1.47</v>
+      </c>
+      <c r="G1827">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:7">
+      <c r="A1828" s="1" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B1828">
+        <v>124</v>
+      </c>
+      <c r="C1828">
+        <v>139.6</v>
+      </c>
+      <c r="D1828">
+        <v>150.8</v>
+      </c>
+      <c r="E1828">
+        <v>161.66</v>
+      </c>
+      <c r="F1828">
+        <v>1.71</v>
+      </c>
+      <c r="G1828">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:7">
+      <c r="A1829" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B1829">
+        <v>119.5</v>
+      </c>
+      <c r="C1829">
+        <v>137.25</v>
+      </c>
+      <c r="D1829">
+        <v>149.25</v>
+      </c>
+      <c r="E1829">
+        <v>160.67</v>
+      </c>
+      <c r="F1829">
+        <v>1.8</v>
+      </c>
+      <c r="G1829">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="1830" spans="1:7">
+      <c r="A1830" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B1830">
+        <v>120</v>
+      </c>
+      <c r="C1830">
+        <v>134.82</v>
+      </c>
+      <c r="D1830">
+        <v>147.7</v>
+      </c>
+      <c r="E1830">
+        <v>159.71</v>
+      </c>
+      <c r="F1830">
+        <v>2.1</v>
+      </c>
+      <c r="G1830">
+        <v>1.14</v>
+      </c>
+    </row>
+    <row r="1831" spans="1:7">
+      <c r="A1831" s="1" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B1831">
+        <v>116</v>
+      </c>
+      <c r="C1831">
+        <v>132.05</v>
+      </c>
+      <c r="D1831">
+        <v>146.03</v>
+      </c>
+      <c r="E1831">
+        <v>158.67</v>
+      </c>
+      <c r="F1831">
+        <v>1.43</v>
+      </c>
+      <c r="G1831">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="1832" spans="1:7">
+      <c r="A1832" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B1832">
+        <v>119.5</v>
+      </c>
+      <c r="C1832">
+        <v>130.19</v>
+      </c>
+      <c r="D1832">
+        <v>144.48</v>
+      </c>
+      <c r="E1832">
+        <v>157.69</v>
+      </c>
+      <c r="F1832">
+        <v>1.29</v>
+      </c>
+      <c r="G1832">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="1833" spans="1:7">
+      <c r="A1833" s="1" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B1833">
+        <v>122.5</v>
+      </c>
+      <c r="C1833">
+        <v>128.53</v>
+      </c>
+      <c r="D1833">
+        <v>143.07</v>
+      </c>
+      <c r="E1833">
+        <v>156.75</v>
+      </c>
+      <c r="F1833">
+        <v>1.15</v>
+      </c>
+      <c r="G1833">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="1834" spans="1:7">
+      <c r="A1834" s="1" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B1834">
+        <v>123</v>
+      </c>
+      <c r="C1834">
+        <v>127.07</v>
+      </c>
+      <c r="D1834">
+        <v>141.73</v>
+      </c>
+      <c r="E1834">
+        <v>155.88</v>
+      </c>
+      <c r="F1834">
+        <v>0.87</v>
+      </c>
+      <c r="G1834">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="1835" spans="1:7">
+      <c r="A1835" s="1" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B1835">
+        <v>124</v>
+      </c>
+      <c r="C1835">
+        <v>125.97</v>
+      </c>
+      <c r="D1835">
+        <v>140.53</v>
+      </c>
+      <c r="E1835">
+        <v>155.03</v>
+      </c>
+      <c r="F1835">
+        <v>0.7</v>
+      </c>
+      <c r="G1835">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="1836" spans="1:7">
+      <c r="A1836" s="1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B1836">
+        <v>126</v>
+      </c>
+      <c r="C1836">
+        <v>125.1</v>
+      </c>
+      <c r="D1836">
+        <v>139.33</v>
+      </c>
+      <c r="E1836">
+        <v>154.22</v>
+      </c>
+      <c r="F1836">
+        <v>0.4</v>
+      </c>
+      <c r="G1836">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="1837" spans="1:7">
+      <c r="A1837" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="B1837">
+        <v>126</v>
+      </c>
+      <c r="C1837">
+        <v>124.6</v>
+      </c>
+      <c r="D1837">
+        <v>138.08</v>
+      </c>
+      <c r="E1837">
+        <v>153.32</v>
+      </c>
+      <c r="F1837">
+        <v>0.24</v>
+      </c>
+      <c r="G1837">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="1838" spans="1:7">
+      <c r="A1838" s="1" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B1838">
+        <v>126</v>
+      </c>
+      <c r="C1838">
+        <v>124.3</v>
+      </c>
+      <c r="D1838">
+        <v>136.93</v>
+      </c>
+      <c r="E1838">
+        <v>152.4</v>
+      </c>
+      <c r="F1838">
+        <v>0.14</v>
+      </c>
+      <c r="G1838">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="1839" spans="1:7">
+      <c r="A1839" s="1" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B1839">
+        <v>127</v>
+      </c>
+      <c r="C1839">
+        <v>124.13</v>
+      </c>
+      <c r="D1839">
+        <v>135.87</v>
+      </c>
+      <c r="E1839">
+        <v>151.6</v>
+      </c>
+      <c r="F1839">
+        <v>0.13</v>
+      </c>
+      <c r="G1839">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="1840" spans="1:7">
+      <c r="A1840" s="1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B1840">
+        <v>128</v>
+      </c>
+      <c r="C1840">
+        <v>123.97</v>
+      </c>
+      <c r="D1840">
+        <v>134.8</v>
+      </c>
+      <c r="E1840">
+        <v>150.75</v>
+      </c>
+      <c r="F1840">
+        <v>0.03</v>
+      </c>
+      <c r="G1840">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="1841" spans="1:7">
+      <c r="A1841" s="1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="B1841">
+        <v>129</v>
+      </c>
+      <c r="C1841">
+        <v>123.93</v>
+      </c>
+      <c r="D1841">
+        <v>133.8</v>
+      </c>
+      <c r="E1841">
+        <v>149.95</v>
+      </c>
+      <c r="F1841">
+        <v>-0.24</v>
+      </c>
+      <c r="G1841">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="1842" spans="1:7">
+      <c r="A1842" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B1842">
+        <v>133</v>
+      </c>
+      <c r="C1842">
+        <v>124.23</v>
+      </c>
+      <c r="D1842">
+        <v>132.94</v>
+      </c>
+      <c r="E1842">
+        <v>149.18</v>
+      </c>
+      <c r="F1842">
+        <v>-0.8</v>
+      </c>
+      <c r="G1842">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:7">
+      <c r="A1843" s="1" t="s">
+        <v>1837</v>
+      </c>
+      <c r="B1843">
+        <v>139</v>
+      </c>
+      <c r="C1843">
+        <v>125.23</v>
+      </c>
+      <c r="D1843">
+        <v>132.42</v>
+      </c>
+      <c r="E1843">
+        <v>148.58</v>
+      </c>
+      <c r="F1843">
+        <v>-1.29</v>
+      </c>
+      <c r="G1843">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="1844" spans="1:7">
+      <c r="A1844" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B1844">
+        <v>144</v>
+      </c>
+      <c r="C1844">
+        <v>126.87</v>
+      </c>
+      <c r="D1844">
+        <v>132.06</v>
+      </c>
+      <c r="E1844">
+        <v>148.07</v>
+      </c>
+      <c r="F1844">
+        <v>-1.4</v>
+      </c>
+      <c r="G1844">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="1845" spans="1:7">
+      <c r="A1845" s="1" t="s">
+        <v>1839</v>
+      </c>
+      <c r="B1845">
+        <v>147</v>
+      </c>
+      <c r="C1845">
+        <v>128.67</v>
+      </c>
+      <c r="D1845">
+        <v>131.74</v>
+      </c>
+      <c r="E1845">
+        <v>147.6</v>
+      </c>
+      <c r="F1845">
+        <v>-1.53</v>
+      </c>
+      <c r="G1845">
+        <v>0.29</v>
+      </c>
+    </row>
+    <row r="1846" spans="1:7">
+      <c r="A1846" s="1" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B1846">
+        <v>146</v>
+      </c>
+      <c r="C1846">
+        <v>130.67</v>
+      </c>
+      <c r="D1846">
+        <v>131.36</v>
+      </c>
+      <c r="E1846">
+        <v>147.12</v>
+      </c>
+      <c r="F1846">
+        <v>-1.33</v>
+      </c>
+      <c r="G1846">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="1847" spans="1:7">
+      <c r="A1847" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B1847">
+        <v>146</v>
+      </c>
+      <c r="C1847">
+        <v>132.43</v>
+      </c>
+      <c r="D1847">
+        <v>131.31</v>
+      </c>
+      <c r="E1847">
+        <v>146.67</v>
+      </c>
+      <c r="F1847">
+        <v>-1.17</v>
+      </c>
+      <c r="G1847">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:7">
+      <c r="A1848" s="1" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B1848">
+        <v>146</v>
+      </c>
+      <c r="C1848">
+        <v>134</v>
+      </c>
+      <c r="D1848">
+        <v>131.27</v>
+      </c>
+      <c r="E1848">
+        <v>146.17</v>
+      </c>
+      <c r="F1848">
+        <v>-1.18</v>
+      </c>
+      <c r="G1848">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="1849" spans="1:7">
+      <c r="A1849" s="1" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B1849">
+        <v>147</v>
+      </c>
+      <c r="C1849">
+        <v>135.6</v>
+      </c>
+      <c r="D1849">
+        <v>131.33</v>
+      </c>
+      <c r="E1849">
+        <v>145.77</v>
+      </c>
+      <c r="F1849">
+        <v>-1.07</v>
+      </c>
+      <c r="G1849">
+        <v>-0.14</v>
+      </c>
+    </row>
+    <row r="1850" spans="1:7">
+      <c r="A1850" s="1" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B1850">
+        <v>146</v>
+      </c>
+      <c r="C1850">
+        <v>137.07</v>
+      </c>
+      <c r="D1850">
+        <v>131.52</v>
+      </c>
+      <c r="E1850">
+        <v>145.4</v>
+      </c>
+      <c r="F1850">
+        <v>-1.01</v>
+      </c>
+      <c r="G1850">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="1851" spans="1:7">
+      <c r="A1851" s="1" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B1851">
+        <v>147</v>
+      </c>
+      <c r="C1851">
+        <v>138.47</v>
+      </c>
+      <c r="D1851">
+        <v>131.78</v>
+      </c>
+      <c r="E1851">
+        <v>145.12</v>
+      </c>
+      <c r="F1851">
+        <v>-1.09</v>
+      </c>
+      <c r="G1851">
+        <v>-0.39</v>
+      </c>
+    </row>
+    <row r="1852" spans="1:7">
+      <c r="A1852" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B1852">
+        <v>149</v>
+      </c>
+      <c r="C1852">
+        <v>140</v>
+      </c>
+      <c r="D1852">
+        <v>132.3</v>
+      </c>
+      <c r="E1852">
+        <v>144.85</v>
+      </c>
+      <c r="F1852">
+        <v>-1.13</v>
+      </c>
+      <c r="G1852">
+        <v>-0.49</v>
+      </c>
+    </row>
+    <row r="1853" spans="1:7">
+      <c r="A1853" s="1" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B1853">
+        <v>150</v>
+      </c>
+      <c r="C1853">
+        <v>141.6</v>
+      </c>
+      <c r="D1853">
+        <v>132.95</v>
+      </c>
+      <c r="E1853">
+        <v>144.65</v>
+      </c>
+      <c r="F1853">
+        <v>-1.03</v>
+      </c>
+      <c r="G1853">
+        <v>-0.49</v>
+      </c>
+    </row>
+    <row r="1854" spans="1:7">
+      <c r="A1854" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B1854">
+        <v>149</v>
+      </c>
+      <c r="C1854">
+        <v>143.07</v>
+      </c>
+      <c r="D1854">
+        <v>133.6</v>
+      </c>
+      <c r="E1854">
+        <v>144.45</v>
+      </c>
+      <c r="F1854">
+        <v>-0.78</v>
+      </c>
+      <c r="G1854">
+        <v>-0.36</v>
+      </c>
+    </row>
+    <row r="1855" spans="1:7">
+      <c r="A1855" s="1" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B1855">
+        <v>145</v>
+      </c>
+      <c r="C1855">
+        <v>144.2</v>
+      </c>
+      <c r="D1855">
+        <v>134.08</v>
+      </c>
+      <c r="E1855">
+        <v>144.17</v>
+      </c>
+      <c r="F1855">
+        <v>-0.87</v>
+      </c>
+      <c r="G1855">
+        <v>-0.46</v>
+      </c>
+    </row>
+    <row r="1856" spans="1:7">
+      <c r="A1856" s="1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B1856">
+        <v>148</v>
+      </c>
+      <c r="C1856">
+        <v>145.47</v>
+      </c>
+      <c r="D1856">
+        <v>134.7</v>
+      </c>
+      <c r="E1856">
+        <v>143.95</v>
+      </c>
+      <c r="F1856">
+        <v>-0.64</v>
+      </c>
+      <c r="G1856">
+        <v>-0.46</v>
+      </c>
+    </row>
+    <row r="1857" spans="1:7">
+      <c r="A1857" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B1857">
+        <v>147</v>
+      </c>
+      <c r="C1857">
+        <v>146.4</v>
+      </c>
+      <c r="D1857">
+        <v>135.32</v>
+      </c>
+      <c r="E1857">
+        <v>143.71</v>
+      </c>
+      <c r="F1857">
+        <v>-0.5</v>
+      </c>
+      <c r="G1857">
+        <v>-0.63</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:7">
+      <c r="A1858" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B1858">
+        <v>150</v>
+      </c>
+      <c r="C1858">
+        <v>147.13</v>
+      </c>
+      <c r="D1858">
+        <v>136.18</v>
+      </c>
+      <c r="E1858">
+        <v>143.49</v>
+      </c>
+      <c r="F1858">
+        <v>-0.32</v>
+      </c>
+      <c r="G1858">
+        <v>-0.77</v>
+      </c>
+    </row>
+    <row r="1859" spans="1:7">
+      <c r="A1859" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="B1859">
+        <v>151</v>
+      </c>
+      <c r="C1859">
+        <v>147.6</v>
+      </c>
+      <c r="D1859">
+        <v>137.23</v>
+      </c>
+      <c r="E1859">
+        <v>143.24</v>
+      </c>
+      <c r="F1859">
+        <v>-0.14</v>
+      </c>
+      <c r="G1859">
+        <v>-0.72</v>
+      </c>
+    </row>
+    <row r="1860" spans="1:7">
+      <c r="A1860" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B1860">
+        <v>150</v>
+      </c>
+      <c r="C1860">
+        <v>147.8</v>
+      </c>
+      <c r="D1860">
+        <v>138.23</v>
+      </c>
+      <c r="E1860">
+        <v>142.97</v>
+      </c>
+      <c r="F1860">
+        <v>0</v>
+      </c>
+      <c r="G1860">
+        <v>-0.72</v>
+      </c>
+    </row>
+    <row r="1861" spans="1:7">
+      <c r="A1861" s="1" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B1861">
+        <v>146</v>
+      </c>
+      <c r="C1861">
+        <v>147.8</v>
+      </c>
+      <c r="D1861">
+        <v>139.23</v>
+      </c>
+      <c r="E1861">
+        <v>142.63</v>
+      </c>
+      <c r="F1861">
+        <v>-0.05</v>
+      </c>
+      <c r="G1861">
+        <v>-0.66</v>
+      </c>
+    </row>
+    <row r="1862" spans="1:7">
+      <c r="A1862" s="1" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B1862">
+        <v>147</v>
+      </c>
+      <c r="C1862">
+        <v>147.87</v>
+      </c>
+      <c r="D1862">
+        <v>140.15</v>
+      </c>
+      <c r="E1862">
+        <v>142.32</v>
+      </c>
+      <c r="F1862">
+        <v>0.09</v>
+      </c>
+      <c r="G1862">
+        <v>-0.51</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:7">
+      <c r="A1863" s="1" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B1863">
+        <v>144</v>
+      </c>
+      <c r="C1863">
+        <v>147.73</v>
+      </c>
+      <c r="D1863">
+        <v>140.87</v>
+      </c>
+      <c r="E1863">
+        <v>141.97</v>
+      </c>
+      <c r="F1863">
+        <v>0.14</v>
+      </c>
+      <c r="G1863">
+        <v>-0.49</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:7">
+      <c r="A1864" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B1864">
+        <v>144</v>
+      </c>
+      <c r="C1864">
+        <v>147.53</v>
+      </c>
+      <c r="D1864">
+        <v>141.57</v>
+      </c>
+      <c r="E1864">
+        <v>141.65</v>
+      </c>
+      <c r="F1864">
+        <v>0.18</v>
+      </c>
+      <c r="G1864">
+        <v>-0.42</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:7">
+      <c r="A1865" s="1" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B1865">
+        <v>142</v>
+      </c>
+      <c r="C1865">
+        <v>147.27</v>
+      </c>
+      <c r="D1865">
+        <v>142.17</v>
+      </c>
+      <c r="E1865">
+        <v>141.35</v>
+      </c>
+      <c r="F1865">
+        <v>0.1</v>
+      </c>
+      <c r="G1865">
+        <v>-0.44</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:7">
+      <c r="A1866" s="1" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B1866">
+        <v>145</v>
+      </c>
+      <c r="C1866">
+        <v>147.13</v>
+      </c>
+      <c r="D1866">
+        <v>142.8</v>
+      </c>
+      <c r="E1866">
+        <v>141.07</v>
+      </c>
+      <c r="F1866">
+        <v>0.27</v>
+      </c>
+      <c r="G1866">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:7">
+      <c r="A1867" s="1" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B1867">
+        <v>143</v>
+      </c>
+      <c r="C1867">
+        <v>146.73</v>
+      </c>
+      <c r="D1867">
+        <v>143.37</v>
+      </c>
+      <c r="E1867">
+        <v>140.72</v>
+      </c>
+      <c r="F1867">
+        <v>0.45</v>
+      </c>
+      <c r="G1867">
+        <v>-0.32</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:7">
+      <c r="A1868" s="1" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B1868">
+        <v>140</v>
+      </c>
+      <c r="C1868">
+        <v>146.07</v>
+      </c>
+      <c r="D1868">
+        <v>143.83</v>
+      </c>
+      <c r="E1868">
+        <v>140.38</v>
+      </c>
+      <c r="F1868">
+        <v>0.6</v>
+      </c>
+      <c r="G1868">
+        <v>-0.21</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:7">
+      <c r="A1869" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="B1869">
+        <v>136</v>
+      </c>
+      <c r="C1869">
+        <v>145.2</v>
+      </c>
+      <c r="D1869">
+        <v>144.13</v>
+      </c>
+      <c r="E1869">
+        <v>140</v>
+      </c>
+      <c r="F1869">
+        <v>0.55</v>
+      </c>
+      <c r="G1869">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:7">
+      <c r="A1870" s="1" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B1870">
+        <v>133</v>
+      </c>
+      <c r="C1870">
+        <v>144.4</v>
+      </c>
+      <c r="D1870">
+        <v>144.3</v>
+      </c>
+      <c r="E1870">
+        <v>139.55</v>
+      </c>
+      <c r="F1870">
+        <v>0.89</v>
+      </c>
+      <c r="G1870">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:7">
+      <c r="A1871" s="1" t="s">
+        <v>1865</v>
+      </c>
+      <c r="B1871">
+        <v>129</v>
+      </c>
+      <c r="C1871">
+        <v>143.13</v>
+      </c>
+      <c r="D1871">
+        <v>144.3</v>
+      </c>
+      <c r="E1871">
+        <v>139.05</v>
+      </c>
+      <c r="F1871">
+        <v>0.8</v>
+      </c>
+      <c r="G1871">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:7">
+      <c r="A1872" s="1" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B1872">
+        <v>130</v>
+      </c>
+      <c r="C1872">
+        <v>142</v>
+      </c>
+      <c r="D1872">
+        <v>144.2</v>
+      </c>
+      <c r="E1872">
+        <v>138.57</v>
+      </c>
+      <c r="F1872">
+        <v>1.09</v>
+      </c>
+      <c r="G1872">
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="1873" spans="1:7">
+      <c r="A1873" s="1" t="s">
+        <v>1867</v>
+      </c>
+      <c r="B1873">
+        <v>127</v>
+      </c>
+      <c r="C1873">
+        <v>140.47</v>
+      </c>
+      <c r="D1873">
+        <v>143.8</v>
+      </c>
+      <c r="E1873">
+        <v>138.11</v>
+      </c>
+      <c r="F1873">
+        <v>1.25</v>
+      </c>
+      <c r="G1873">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:7">
+      <c r="A1874" s="1" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B1874">
+        <v>125</v>
+      </c>
+      <c r="C1874">
+        <v>138.73</v>
+      </c>
+      <c r="D1874">
+        <v>143.17</v>
+      </c>
+      <c r="E1874">
+        <v>137.61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>